<commit_message>
1. update RB data to 2023-11-23; 2. update analyzing framework
</commit_message>
<xml_diff>
--- a/data/钢铁产业链/中游数据/螺纹钢/螺纹钢产量.xlsx
+++ b/data/钢铁产业链/中游数据/螺纹钢/螺纹钢产量.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Repository\Projects\ffa\data\钢铁产业链\中游数据\螺纹钢\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Document\Project\ffa\data\钢铁产业链\中游数据\螺纹钢\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D361CF92-5D2A-41CE-A9C7-C874ABDA0708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051BEE5A-A6A9-4381-BF45-89FB4D8E809B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="277" windowWidth="38596" windowHeight="20146" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>howard</author>
+    <author>FUDIAN</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7A27921F-9BA0-419E-815F-9A1902F9FDEE}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{F57D6EF2-3498-4198-B97F-4119BB1C2722}">
       <text>
         <r>
           <rPr>
@@ -49,10 +49,9 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>yVjpCgZpNvM+1uqZaQy5fWsnFn5LuXU8wJ48VaigH4pMxhl3I+UVtddn6UsNbNriJq2tF1otd2Quo8ZTJQifLb7TFDK/wb9m0N2ql9M8X77D45oUHbBxYKhTp/YZ5eg8xC46V0a/9fijMO1qKMzIiTYA4IDYJMyLZkGeuDDYZmt2KehVya8aRUcmVGg7KC1Ap3w1cZSWmPkkgtIbs780EE2lQxSgLT5DPoATQveVWCUigTaU5d9r917VQI1cJ1mdvLduPsDdb0wEUx6NSAfiw6VRYRoxEyHvD9qxAjdIEwgmbV0UjBWqMh0VUPfUsQKiHR8/W38QffkriZyPHDaWOP4SYj/x1mcdu2WTkTbw3y7+d3obAUIpXBvX/k3Micwr3bB7Nbv8n3+VWg3lWkTz+6bnFXJ+xX0iMJx90dO8jEVUrIS/Fdx9XM9O4iAgXOxM58xZWxuzeSbDVHNUUz1mwgS+KODVBsHCUiV6mlm91SOLMlUE1r/1yH697RZXi7RHearzcAa2GSlQcEynFU2dJlbBBW7/aNL/z9amLHBxcI9UPujLO4QY3Cfb4Mz0lFVjNis7TJX/4+RMvtd15bQpIjo+mCMa+7OIe0JJpRjB3TZtaD2iUgMxHRXr96H6NnxfQENkW/GaSpkd1QjElKOUl4Mh3a8Wg4pwdaV8jNI8JQ3vSLbUGYArx5FylWlxPumWldkfDM8V7eNlOkXES6zQvMvlF5KSeY7x3ZIDs8+og7TcQcnOrtjQQglEt4yQKTnXbO4aa3Dm2UMO8e5eSSeuxW0J6yzFlzUSF4GC4YqJ8qnnMz6D/3XB9xDp0EwUM315VQHHqc4zAGiwQiywRiwq4G7f8YfJRjZ0Fy8IanxmN5Ea9zJmy6d5/EOErR4yfKmekdy2fRDxDLH5t6195l/kypaVSgyMtd1PENpxIahZSX2/+ODh8dNHyTtFYqQgvmgPh2rAip94llG6LQMeA1Y+nb1hfVsePiVvHlj7mfM3Mz4E+zHldOst2w==</t>
+          <t>yVjpCgZpNvOHlEoAN60+iXcNR8qcjD2afR3U+XlDrUTEX5W5KWYQZl2WlS6znR8JdtRv8fy9hcGzGgX1t8jwbDwAx0EUQZsw3ZWNu8RJYhGO4TcQ9l1JkQHbe3Y9+FG0Tmzb5nAqIClWWKfYkQKr3HY3DNkUELEitQOt11rUEoTH9AyAvxvPtRPK/Y6fy4lz2KWBJYBci5O9pBsPURqiuNGQqyCnjH7Ung5z+ii9hq1rT4vBAzSgen+CCy1rso9qyU/kUkxgP2I7TJPKJc3EhlF7XmdlYP35A5gJCV2fr8qrcy7CkTgPG/VvhJioiSolN7TiUCKuFQ8Qy42CZl736H4MD9NJOTvtLP7OD4DDnztg6nQG+IRT3vc1XCoMdmCFo5mcYda9mfh2zr59msXjahKRvnoXUzFH9fOiToc9t1oRkkLFXDo56rxU/05E/nOguyWkk7HUVMOijhgJr/dueZpcPHS6QP+Cr+Ugsvtzs1jX2S5V+C2SyJETu5ba2RUwAHlpAQ56ZlrL1ONsyC8VOasoczKjsO8ZSm/h84r6VFyN4h0MJvJKOENrnW8TMAqegj+Ua71zT/jgcUiWrAvEUtuuu5BrVk/R+5pRll3U12/WRffPXBXTWa2bJ6fgsfXNdCqpNt6VAp4w8LjqOc8dKHx3DYn8rZftq+FohR+YM8g8MzKMR9XQGPia6FqQGWjeCVouf2mI+/opLJJ+X00amgXThZr9itdrA4YpS7rODF5aJ/MNS+GJxh56sQiyscV/xOS+Hji9YMoNQwhd9fwMDCXSC6jK3qQ2+VRzkD7Sway9uTam/kr1RwzNGfY/SvK6dIDwEnQ0fjT+RyyLewLGzLfDpuZTh+E1HZKPBVIhRzsWtwrrhhakZK2DocBd74wDT36lUilCNOhaEawPHg0iE8me7bgWQs9tziasPs/zQH10oTFpE7j0DW1IagjVScMbwjvIahEGDLYkyU0gmmF2xaQa0DMr1ko1Sd5gaekPoz4KZf2oYXMTQJAovidrwTRJtXOEMKFfjFFBPuZAApCS3KCsK/kckUgRy25SldNziSqqf8HbCheP5Udqn0haOazV/bmj/pf+M75gXAT5OuY5wV1lbu8s9Z0OFfRictVCY8WjeOLrJsJQu5uMvPTPgps7hD5QO/rocHld9gGMeYHDx4xk1Z6kZ6JfX9er55eGk8dWX8RkEZNiDoBrAiPfKrOYtgkQwOP7f6+xLbBwl5OUVlqw5ha4suXfMwleLFIMVj0cGkw8oPHhN+2HP9CXFxVJ0gA5e0Q4glR8tS6Vsn1tf/xjQ8F+bl9tangNKNDPMsYWF2ngs89a/cspZfdVG4FQCOdatToTRF7xjhnQLnXhf02LPi0m6g1rgj3qkEGns5NKZL1yEy5xufbBhmx6XcshyAB2O/KS6a0SqKx2P9NiVN2IYwh7jpTakjRsMkd2736r00WgHT3LUnLH9EJ/NXzvtr1CRU9LVL8fkDe+8KLICBGuclobMzmI</t>
         </r>
       </text>
     </comment>
@@ -110,7 +109,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -138,14 +137,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -168,6 +159,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="6">
@@ -241,16 +239,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -755,26 +753,26 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
       <selection activeCell="E161" sqref="E161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="str">
         <f>[1]!EM_EDB_N("2010-3-29","N","Columns=Name,Frequency,Unit,Source&amp;Order=2&amp;DateFormat=1&amp;Chart=2&amp;ClearArea=NULL&amp;CellFormat=1&amp;Layout=0")</f>
         <v>宏观数据</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -791,7 +789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -808,7 +806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -825,7 +823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -842,7 +840,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>40268</v>
       </c>
@@ -859,7 +857,7 @@
         <v>14.82431467</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>40298</v>
       </c>
@@ -876,7 +874,7 @@
         <v>15.998117580000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
         <v>40329</v>
       </c>
@@ -893,7 +891,7 @@
         <v>16.894170450000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5">
         <v>40359</v>
       </c>
@@ -910,7 +908,7 @@
         <v>13.69273102</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
         <v>40390</v>
       </c>
@@ -927,7 +925,7 @@
         <v>12.09851177</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5">
         <v>40421</v>
       </c>
@@ -944,7 +942,7 @@
         <v>11.06826083</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5">
         <v>40451</v>
       </c>
@@ -961,7 +959,7 @@
         <v>10.43715055</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5">
         <v>40482</v>
       </c>
@@ -978,7 +976,7 @@
         <v>8.7005333700000005</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5">
         <v>40512</v>
       </c>
@@ -995,7 +993,7 @@
         <v>7.0415532000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5">
         <v>40543</v>
       </c>
@@ -1012,7 +1010,7 @@
         <v>7.7833414000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5">
         <v>40574</v>
       </c>
@@ -1029,7 +1027,7 @@
         <v>11.040897810000001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5">
         <v>40602</v>
       </c>
@@ -1046,7 +1044,7 @@
         <v>14.183199999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5">
         <v>40633</v>
       </c>
@@ -1063,7 +1061,7 @@
         <v>13.799099999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5">
         <v>40663</v>
       </c>
@@ -1080,7 +1078,7 @@
         <v>12.631500000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5">
         <v>40694</v>
       </c>
@@ -1097,7 +1095,7 @@
         <v>12.9131</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5">
         <v>40724</v>
       </c>
@@ -1114,7 +1112,7 @@
         <v>15.1815</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5">
         <v>40755</v>
       </c>
@@ -1131,7 +1129,7 @@
         <v>16.718699999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5">
         <v>40786</v>
       </c>
@@ -1148,7 +1146,7 @@
         <v>17.6069</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5">
         <v>40816</v>
       </c>
@@ -1165,7 +1163,7 @@
         <v>18.717300000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5">
         <v>40847</v>
       </c>
@@ -1182,7 +1180,7 @@
         <v>19.047599999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5">
         <v>40877</v>
       </c>
@@ -1199,7 +1197,7 @@
         <v>19.038599999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="5">
         <v>40908</v>
       </c>
@@ -1216,7 +1214,7 @@
         <v>18.007300000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5">
         <v>40939</v>
       </c>
@@ -1233,7 +1231,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5">
         <v>40968</v>
       </c>
@@ -1250,7 +1248,7 @@
         <v>12.891500000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5">
         <v>40999</v>
       </c>
@@ -1267,7 +1265,7 @@
         <v>16.413</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="5">
         <v>41029</v>
       </c>
@@ -1284,7 +1282,7 @@
         <v>15.1637</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5">
         <v>41060</v>
       </c>
@@ -1301,7 +1299,7 @@
         <v>14.3429</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="5">
         <v>41090</v>
       </c>
@@ -1318,7 +1316,7 @@
         <v>13.945600000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="5">
         <v>41121</v>
       </c>
@@ -1335,7 +1333,7 @@
         <v>13.7437</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5">
         <v>41152</v>
       </c>
@@ -1352,7 +1350,7 @@
         <v>12.8962</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5">
         <v>41182</v>
       </c>
@@ -1369,7 +1367,7 @@
         <v>13.867000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="5">
         <v>41213</v>
       </c>
@@ -1386,7 +1384,7 @@
         <v>14.8561</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5">
         <v>41243</v>
       </c>
@@ -1403,7 +1401,7 @@
         <v>15.530654999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5">
         <v>41274</v>
       </c>
@@ -1420,7 +1418,7 @@
         <v>14.95</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5">
         <v>41333</v>
       </c>
@@ -1433,7 +1431,7 @@
         <v>16.896106769999999</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5">
         <v>41364</v>
       </c>
@@ -1450,7 +1448,7 @@
         <v>12.06963236</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="5">
         <v>41394</v>
       </c>
@@ -1467,7 +1465,7 @@
         <v>12.830299249999999</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="5">
         <v>41425</v>
       </c>
@@ -1484,7 +1482,7 @@
         <v>13.18038634</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="5">
         <v>41455</v>
       </c>
@@ -1501,7 +1499,7 @@
         <v>13.11549817</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="5">
         <v>41486</v>
       </c>
@@ -1518,7 +1516,7 @@
         <v>13.300737829999999</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="5">
         <v>41517</v>
       </c>
@@ -1535,7 +1533,7 @@
         <v>13.928129370000001</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="5">
         <v>41547</v>
       </c>
@@ -1552,7 +1550,7 @@
         <v>13.663710180000001</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="5">
         <v>41578</v>
       </c>
@@ -1569,7 +1567,7 @@
         <v>13.318869530000001</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="5">
         <v>41608</v>
       </c>
@@ -1586,7 +1584,7 @@
         <v>13.056521589999999</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="5">
         <v>41639</v>
       </c>
@@ -1603,7 +1601,7 @@
         <v>13.802464540000001</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="5">
         <v>41698</v>
       </c>
@@ -1616,7 +1614,7 @@
         <v>13.83075644</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="5">
         <v>41729</v>
       </c>
@@ -1633,7 +1631,7 @@
         <v>9.5536193699999998</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="5">
         <v>41759</v>
       </c>
@@ -1650,7 +1648,7 @@
         <v>9.5997613400000006</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="5">
         <v>41790</v>
       </c>
@@ -1667,7 +1665,7 @@
         <v>10.259932750000001</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="5">
         <v>41820</v>
       </c>
@@ -1684,7 +1682,7 @@
         <v>10.762424409999999</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="5">
         <v>41851</v>
       </c>
@@ -1701,7 +1699,7 @@
         <v>8.7776094400000009</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="5">
         <v>41882</v>
       </c>
@@ -1718,7 +1716,7 @@
         <v>7.6913239500000001</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="5">
         <v>41912</v>
       </c>
@@ -1735,7 +1733,7 @@
         <v>7.0604863</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="5">
         <v>41943</v>
       </c>
@@ -1752,7 +1750,7 @@
         <v>6.5797384799999996</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="5">
         <v>41973</v>
       </c>
@@ -1769,7 +1767,7 @@
         <v>6.0966545999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="5">
         <v>42004</v>
       </c>
@@ -1786,7 +1784,7 @@
         <v>4.7722927200000003</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="5">
         <v>42063</v>
       </c>
@@ -1799,7 +1797,7 @@
         <v>-4.9741966499999997</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="5">
         <v>42094</v>
       </c>
@@ -1816,7 +1814,7 @@
         <v>-3.3665035699999999</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="5">
         <v>42124</v>
       </c>
@@ -1833,7 +1831,7 @@
         <v>-3.5897998000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="5">
         <v>42155</v>
       </c>
@@ -1850,7 +1848,7 @@
         <v>-3.9814830799999998</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="5">
         <v>42185</v>
       </c>
@@ -1867,7 +1865,7 @@
         <v>-3.8827965400000002</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="5">
         <v>42216</v>
       </c>
@@ -1884,7 +1882,7 @@
         <v>-4.9728593099999996</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="5">
         <v>42247</v>
       </c>
@@ -1901,7 +1899,7 @@
         <v>-4.7385967999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="5">
         <v>42277</v>
       </c>
@@ -1918,7 +1916,7 @@
         <v>-3.94796287</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="5">
         <v>42308</v>
       </c>
@@ -1935,7 +1933,7 @@
         <v>-4.0363945599999997</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="5">
         <v>42338</v>
       </c>
@@ -1952,7 +1950,7 @@
         <v>-3.7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="5">
         <v>42369</v>
       </c>
@@ -1969,7 +1967,7 @@
         <v>-3.5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="5">
         <v>42429</v>
       </c>
@@ -1982,7 +1980,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="5">
         <v>42460</v>
       </c>
@@ -1999,7 +1997,7 @@
         <v>-3.6</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="5">
         <v>42490</v>
       </c>
@@ -2016,7 +2014,7 @@
         <v>-2.6</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="5">
         <v>42521</v>
       </c>
@@ -2033,7 +2031,7 @@
         <v>-1.4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="5">
         <v>42551</v>
       </c>
@@ -2050,7 +2048,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="5">
         <v>42582</v>
       </c>
@@ -2067,7 +2065,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="5">
         <v>42613</v>
       </c>
@@ -2084,7 +2082,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="5">
         <v>42643</v>
       </c>
@@ -2101,7 +2099,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="5">
         <v>42674</v>
       </c>
@@ -2118,7 +2116,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="5">
         <v>42704</v>
       </c>
@@ -2135,7 +2133,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="5">
         <v>42735</v>
       </c>
@@ -2152,7 +2150,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="5">
         <v>42794</v>
       </c>
@@ -2165,7 +2163,7 @@
         <v>-2.7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="5">
         <v>42825</v>
       </c>
@@ -2182,7 +2180,7 @@
         <v>-3.5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="5">
         <v>42855</v>
       </c>
@@ -2199,7 +2197,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="5">
         <v>42886</v>
       </c>
@@ -2216,7 +2214,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="5">
         <v>42916</v>
       </c>
@@ -2233,7 +2231,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="5">
         <v>42947</v>
       </c>
@@ -2250,7 +2248,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="5">
         <v>42978</v>
       </c>
@@ -2267,7 +2265,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="5">
         <v>43008</v>
       </c>
@@ -2284,7 +2282,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="5">
         <v>43039</v>
       </c>
@@ -2301,7 +2299,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="5">
         <v>43069</v>
       </c>
@@ -2318,7 +2316,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="5">
         <v>43100</v>
       </c>
@@ -2335,7 +2333,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="5">
         <v>43159</v>
       </c>
@@ -2348,7 +2346,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="5">
         <v>43190</v>
       </c>
@@ -2365,7 +2363,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="5">
         <v>43220</v>
       </c>
@@ -2382,7 +2380,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="5">
         <v>43251</v>
       </c>
@@ -2399,7 +2397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="5">
         <v>43281</v>
       </c>
@@ -2416,7 +2414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="5">
         <v>43312</v>
       </c>
@@ -2433,7 +2431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="5">
         <v>43343</v>
       </c>
@@ -2450,7 +2448,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="5">
         <v>43373</v>
       </c>
@@ -2467,7 +2465,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="5">
         <v>43404</v>
       </c>
@@ -2484,7 +2482,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="5">
         <v>43434</v>
       </c>
@@ -2501,7 +2499,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="5">
         <v>43465</v>
       </c>
@@ -2518,7 +2516,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="5">
         <v>43524</v>
       </c>
@@ -2531,7 +2529,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="5">
         <v>43555</v>
       </c>
@@ -2548,7 +2546,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="5">
         <v>43585</v>
       </c>
@@ -2565,7 +2563,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="5">
         <v>43616</v>
       </c>
@@ -2582,7 +2580,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="5">
         <v>43646</v>
       </c>
@@ -2599,7 +2597,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="5">
         <v>43677</v>
       </c>
@@ -2616,7 +2614,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="5">
         <v>43708</v>
       </c>
@@ -2633,7 +2631,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="5">
         <v>43738</v>
       </c>
@@ -2650,7 +2648,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="5">
         <v>43769</v>
       </c>
@@ -2667,7 +2665,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="5">
         <v>43799</v>
       </c>
@@ -2684,7 +2682,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="5">
         <v>43830</v>
       </c>
@@ -2701,7 +2699,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="5">
         <v>43890</v>
       </c>
@@ -2714,7 +2712,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="5">
         <v>43921</v>
       </c>
@@ -2731,7 +2729,7 @@
         <v>-1.9</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="5">
         <v>43951</v>
       </c>
@@ -2748,7 +2746,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="5">
         <v>43982</v>
       </c>
@@ -2765,7 +2763,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="5">
         <v>44012</v>
       </c>
@@ -2782,7 +2780,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="5">
         <v>44043</v>
       </c>
@@ -2799,7 +2797,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="5">
         <v>44074</v>
       </c>
@@ -2816,7 +2814,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="5">
         <v>44104</v>
       </c>
@@ -2833,7 +2831,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="5">
         <v>44135</v>
       </c>
@@ -2850,7 +2848,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="5">
         <v>44165</v>
       </c>
@@ -2867,7 +2865,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="5">
         <v>44196</v>
       </c>
@@ -2884,7 +2882,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="5">
         <v>44255</v>
       </c>
@@ -2897,7 +2895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="5">
         <v>44286</v>
       </c>
@@ -2914,7 +2912,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="5">
         <v>44316</v>
       </c>
@@ -2931,7 +2929,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="5">
         <v>44347</v>
       </c>
@@ -2948,7 +2946,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="5">
         <v>44377</v>
       </c>
@@ -2965,7 +2963,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="5">
         <v>44408</v>
       </c>
@@ -2982,7 +2980,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="5">
         <v>44439</v>
       </c>
@@ -2999,7 +2997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="5">
         <v>44469</v>
       </c>
@@ -3016,7 +3014,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="5">
         <v>44500</v>
       </c>
@@ -3033,7 +3031,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="5">
         <v>44530</v>
       </c>
@@ -3050,7 +3048,7 @@
         <v>-4.0999999999999996</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="5">
         <v>44561</v>
       </c>
@@ -3067,7 +3065,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="5">
         <v>44620</v>
       </c>
@@ -3080,7 +3078,7 @@
         <v>-13.8</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="5">
         <v>44651</v>
       </c>
@@ -3097,7 +3095,7 @@
         <v>-13.3</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="5">
         <v>44681</v>
       </c>
@@ -3114,7 +3112,7 @@
         <v>-13.6</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="5">
         <v>44712</v>
       </c>
@@ -3131,7 +3129,7 @@
         <v>-12.9</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="5">
         <v>44742</v>
       </c>
@@ -3148,7 +3146,7 @@
         <v>-14.1</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="5">
         <v>44773</v>
       </c>
@@ -3165,7 +3163,7 @@
         <v>-14.7</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="5">
         <v>44804</v>
       </c>
@@ -3182,7 +3180,7 @@
         <v>-13.8</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="5">
         <v>44834</v>
       </c>
@@ -3199,7 +3197,7 @@
         <v>-11.1</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" s="5">
         <v>44865</v>
       </c>
@@ -3216,7 +3214,7 @@
         <v>-9.5</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="5">
         <v>44895</v>
       </c>
@@ -3233,7 +3231,7 @@
         <v>-8.1</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="5">
         <v>44926</v>
       </c>
@@ -3250,7 +3248,7 @@
         <v>-8.1</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A150" s="5">
         <v>44985</v>
       </c>
@@ -3263,7 +3261,7 @@
         <v>-4.7</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A151" s="5">
         <v>45016</v>
       </c>
@@ -3280,7 +3278,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A152" s="5">
         <v>45046</v>
       </c>
@@ -3297,7 +3295,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A153" s="5">
         <v>45077</v>
       </c>
@@ -3314,7 +3312,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A154" s="5">
         <v>45107</v>
       </c>
@@ -3331,7 +3329,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A155" s="5">
         <v>45138</v>
       </c>
@@ -3348,7 +3346,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A156" s="5">
         <v>45169</v>
       </c>
@@ -3365,7 +3363,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A157" s="5">
         <v>45199</v>
       </c>
@@ -3382,7 +3380,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A158" s="5">
         <v>45230</v>
       </c>
@@ -3399,18 +3397,18 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A160" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A161" s="2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>